<commit_message>
Algumas pequenas alterações para a entrega do Lab4
</commit_message>
<xml_diff>
--- a/Instruções.xlsx
+++ b/Instruções.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ArqComp\ProjetoMicroProcessador\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF429022-2839-4AFA-820D-FF8C1CE3D4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Instruções</t>
+  </si>
+  <si>
+    <t>num de bits: 18</t>
+  </si>
+  <si>
+    <t>formato</t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>[reserv17:13|end12:6|func5:4|op3:0]</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>vetor</t>
+  </si>
+  <si>
+    <t>func:00,op:1111</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +374,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Começo do Lab5, feito o extensor de sinal, adicionado 4 estados na UC e o registrador de instrução
</commit_message>
<xml_diff>
--- a/Instruções.xlsx
+++ b/Instruções.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ArqComp\ProjetoMicroProcessador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF429022-2839-4AFA-820D-FF8C1CE3D4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BFA93B-E27F-44A8-BDE1-4537A6DC6264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Instruções</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Jump</t>
   </si>
   <si>
-    <t>[reserv17:13|end12:6|func5:4|op3:0]</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -54,15 +51,101 @@
     <t>vetor</t>
   </si>
   <si>
-    <t>func:00,op:1111</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>func:00,op:111</t>
+  </si>
+  <si>
+    <t>func:00,op:000</t>
+  </si>
+  <si>
+    <t>[reserv17:12|end11:5|func4:3|op2:0]</t>
+  </si>
+  <si>
+    <t>[zeros17:5|func4:3|op2:0]</t>
+  </si>
+  <si>
+    <t>Nop</t>
+  </si>
+  <si>
+    <t>Ld</t>
+  </si>
+  <si>
+    <t>acc &lt;- const</t>
+  </si>
+  <si>
+    <t>Rn &lt;- const</t>
+  </si>
+  <si>
+    <t>func:00,op:001</t>
+  </si>
+  <si>
+    <t>func:01,op:001</t>
+  </si>
+  <si>
+    <t>Mov</t>
+  </si>
+  <si>
+    <t>A&lt;-Rn</t>
+  </si>
+  <si>
+    <t>func:00,op:010</t>
+  </si>
+  <si>
+    <t>func:01,op:010</t>
+  </si>
+  <si>
+    <t>Rn&lt;-A</t>
+  </si>
+  <si>
+    <t>op(tipo)</t>
+  </si>
+  <si>
+    <t>Rn &lt;-A</t>
+  </si>
+  <si>
+    <t>func:00 soma op:011</t>
+  </si>
+  <si>
+    <t>func:01 Subtração op:011</t>
+  </si>
+  <si>
+    <t>func:00 Nand op:011</t>
+  </si>
+  <si>
+    <t>func:00 Xor op:011</t>
+  </si>
+  <si>
+    <t>[const17:11|tipo10:9|rn8:6|acc5|func4:3|op2:0]</t>
+  </si>
+  <si>
+    <t>[const17:11|reservado10:6|acc5|func4:3|op2:0]</t>
+  </si>
+  <si>
+    <t>[const17:11|reservado10:8|rn7:5|func4:3|op2:0]</t>
+  </si>
+  <si>
+    <t>[const17:11|reservado10:9|rn8:6|acc5|func4:3|op2:0]</t>
+  </si>
+  <si>
+    <t>[const17:11?|reservado10:9|rn8:6|acc5|func4:3|op2:0]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,11 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="141" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,7 +470,7 @@
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
     <col min="2" max="2" width="33.88671875" customWidth="1"/>
     <col min="3" max="3" width="35.21875" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="4" max="4" width="49.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -407,16 +491,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -424,13 +508,139 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -439,5 +649,6 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>